<commit_message>
Refix ZSS-944: change column width should relayout 90deg rotate text.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/944-90deg-text.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/944-90deg-text.xlsx
@@ -16,62 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="2">
   <si>
-    <t>deg-90 v-top h-left</t>
+    <t>This is a test</t>
   </si>
   <si>
-    <t>deg-90 v-top h-center</t>
-  </si>
-  <si>
-    <t>deg-90 v-top h-right</t>
-  </si>
-  <si>
-    <t>deg90 v-top h-left</t>
-  </si>
-  <si>
-    <t>deg90 v-top h-right</t>
-  </si>
-  <si>
-    <t>deg90 v-center h-left</t>
-  </si>
-  <si>
-    <t>deg90 v-center h-center</t>
-  </si>
-  <si>
-    <t>deg90 v-center h-right</t>
-  </si>
-  <si>
-    <t>deg-90 v-center h-left</t>
-  </si>
-  <si>
-    <t>deg90 v-bottom h-left</t>
-  </si>
-  <si>
-    <t>deg90 v-bottom h-center</t>
-  </si>
-  <si>
-    <t>deg90 v-bottom h-right</t>
-  </si>
-  <si>
-    <t>deg-90 v-bottom h-left</t>
-  </si>
-  <si>
-    <t>deg-90 v-center h-center</t>
-  </si>
-  <si>
-    <t>deg-90 v-center h-right</t>
-  </si>
-  <si>
-    <t>deg-90 v-bottom h-center</t>
-  </si>
-  <si>
-    <t>deg-90 v-bottom h-right</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">deg90 </t>
-    </r>
     <r>
       <rPr>
         <sz val="14"/>
@@ -80,7 +29,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>v-top</t>
+      <t>This</t>
     </r>
     <r>
       <rPr>
@@ -90,7 +39,57 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> h-center</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
     </r>
   </si>
 </sst>
@@ -98,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +115,27 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,12 +231,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" textRotation="180"/>
     </xf>
@@ -258,6 +272,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,7 +576,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,61 +585,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="170.25" customHeight="1">
-      <c r="A1" s="18" t="s">
-        <v>3</v>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="170.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>16</v>
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>